<commit_message>
Docker implemented with db
</commit_message>
<xml_diff>
--- a/IDVerification/IDVerification/Documents/FATF_Jurisdiction_Ratings xlsx.xlsx
+++ b/IDVerification/IDVerification/Documents/FATF_Jurisdiction_Ratings xlsx.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Data!$A$1:$G$105</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Data!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Data!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Data!$A$1:$G$105</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,22 +26,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="123">
   <si>
-    <t xml:space="preserve">JurisdictionId</t>
+    <t xml:space="preserve">Id</t>
   </si>
   <si>
     <t xml:space="preserve">Jurisdiction</t>
   </si>
   <si>
-    <t xml:space="preserve">EffectivenessScore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CountryEffectivenessRating</t>
+    <t xml:space="preserve">EffectiveScore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CountryEffectiveRating</t>
   </si>
   <si>
     <t xml:space="preserve">TechnicalComplianceScore</t>
   </si>
   <si>
-    <t xml:space="preserve">TechnicalComplianceTcRating</t>
+    <t xml:space="preserve">TechnicalComplianceRating</t>
   </si>
   <si>
     <t xml:space="preserve">Comments</t>
@@ -402,7 +402,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -423,6 +423,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <color rgb="FF000000"/>
+      <name val="Cascadia Mono"/>
       <family val="0"/>
     </font>
     <font>
@@ -475,12 +481,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -508,10 +518,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TBL_Employees" displayName="TBL_Employees" ref="A1:D105" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A1:D105"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="JurisdictionId"/>
+    <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Jurisdiction"/>
-    <tableColumn id="3" name="EffectivenessScore"/>
-    <tableColumn id="4" name="CountryEffectivenessRating"/>
+    <tableColumn id="3" name="EffectiveScore"/>
+    <tableColumn id="4" name="CountryEffectiveRating"/>
   </tableColumns>
 </table>
 </file>
@@ -524,7 +534,7 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -540,11 +550,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1015" style="0" width="11.57"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -559,7 +569,7 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3909,7 +3919,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:G105"/>
+  <autoFilter ref="A1:G1"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>